<commit_message>
2024-01-15 draft and summaries progress
</commit_message>
<xml_diff>
--- a/src/data/raw/2024-01-09_review_papers.xlsx
+++ b/src/data/raw/2024-01-09_review_papers.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lex/Workspace/phd-research-ucc/repositories/mrs-systematic-analysis/src/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5BF31A-81F0-2D46-AC68-4D37F2B7CCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E406DE78-97A3-2640-8617-2D67424AA713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" activeTab="1" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
+    <workbookView xWindow="17980" yWindow="740" windowWidth="16580" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-01-03_review_papers" sheetId="1" r:id="rId1"/>
+    <sheet name="review_papers" sheetId="1" r:id="rId1"/>
     <sheet name="research_methods" sheetId="9" r:id="rId2"/>
     <sheet name="source_refs" sheetId="8" r:id="rId3"/>
     <sheet name="search_dbs" sheetId="5" r:id="rId4"/>
@@ -1330,6 +1330,12 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1337,12 +1343,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1825,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068F48D0-C0F6-0F48-8756-0A46C8000F25}">
   <dimension ref="B2:U40"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3473,6 +3473,9 @@
       </c>
       <c r="C28" t="s">
         <v>331</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
@@ -3899,10 +3902,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N31 N33:N34">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="notEqual">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4063,7 +4066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F018DA4A-F1B8-1241-9B51-86661EAE30B1}">
   <dimension ref="B2:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2024-01-16 import progress in lit review compilation
</commit_message>
<xml_diff>
--- a/src/data/raw/2024-01-09_review_papers.xlsx
+++ b/src/data/raw/2024-01-09_review_papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lex/Workspace/phd-research-ucc/repositories/mrs-systematic-analysis/src/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E406DE78-97A3-2640-8617-2D67424AA713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB3C55-6B27-2644-8B94-04EA24458410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17980" yWindow="740" windowWidth="16580" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
   </bookViews>
   <sheets>
     <sheet name="review_papers" sheetId="1" r:id="rId1"/>
@@ -1248,7 +1248,7 @@
       <alignment horizontal="fill" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1271,9 +1271,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1281,7 +1284,129 @@
     <cellStyle name="Style 1" xfId="2" xr:uid="{AD703E83-2422-144D-99A8-2ADC57964367}"/>
     <cellStyle name="Style 2" xfId="3" xr:uid="{B9FF1B68-E23A-3C40-85DE-B173152847B9}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1330,12 +1455,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1343,6 +1462,12 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1381,6 +1506,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1466,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}" name="Table1" displayName="Table1" ref="B2:U40" totalsRowShown="0">
-  <autoFilter ref="B2:U40" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}" name="Table1" displayName="Table1" ref="B2:U41" totalsRowShown="0">
+  <autoFilter ref="B2:U41" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:U34">
     <sortCondition ref="B2:B34"/>
   </sortState>
@@ -1480,18 +1615,18 @@
     <tableColumn id="7" xr3:uid="{B5956E56-EA0C-C544-81E9-95D5F85516CE}" name="year"/>
     <tableColumn id="8" xr3:uid="{1D433107-5A8B-4B40-8584-1024473C053A}" name="type"/>
     <tableColumn id="9" xr3:uid="{28A710C7-54CD-BC4D-A29E-7C74FFEB5F42}" name="domain"/>
-    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="32"/>
     <tableColumn id="17" xr3:uid="{5A2B4EE5-BF86-7042-97F7-E54C28D22FA9}" name="covid19"/>
-    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="31"/>
     <tableColumn id="19" xr3:uid="{E63FEC1A-8B57-1B47-AAEC-C5489A7E23BF}" name="coi"/>
-    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="30"/>
+    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="29"/>
+    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1501,7 +1636,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}" name="Table2" displayName="Table2" ref="B2:F46" totalsRowShown="0">
   <autoFilter ref="B2:F46" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{E697A4C6-CB50-0449-AD63-6ACBEE53E663}" name="local_ref"/>
     <tableColumn id="3" xr3:uid="{53E59951-C7CE-0740-917C-0D957BB1897C}" name="ref_url"/>
     <tableColumn id="4" xr3:uid="{1E16B457-6000-4743-9439-9D6865E34250}" name="ref_comment"/>
@@ -1823,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068F48D0-C0F6-0F48-8756-0A46C8000F25}">
-  <dimension ref="B2:U40"/>
+  <dimension ref="B2:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2293,82 +2428,35 @@
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>2023</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="K9" s="5">
-        <v>5</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="M9" t="s">
-        <v>183</v>
-      </c>
-      <c r="N9" t="s">
-        <v>185</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>154</v>
-      </c>
-      <c r="R9" t="s">
-        <v>187</v>
-      </c>
-      <c r="S9" t="s">
-        <v>181</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="U9" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="14"/>
+      <c r="P9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="3"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="H10" t="s">
         <v>38</v>
@@ -2377,37 +2465,37 @@
         <v>65</v>
       </c>
       <c r="J10" s="1">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="K10" s="5">
         <v>5</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="M10" t="s">
-        <v>188</v>
-      </c>
-      <c r="N10" t="s">
-        <v>75</v>
+        <v>184</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" t="s">
-        <v>190</v>
+      <c r="P10" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="Q10" t="s">
-        <v>155</v>
-      </c>
-      <c r="R10" t="s">
-        <v>155</v>
-      </c>
-      <c r="S10" t="s">
-        <v>191</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>192</v>
+        <v>154</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="S10" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>69</v>
@@ -2418,58 +2506,58 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="K11" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M11" t="s">
-        <v>193</v>
-      </c>
-      <c r="N11" t="s">
-        <v>197</v>
+        <v>189</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" t="s">
-        <v>196</v>
+      <c r="P11" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="Q11" t="s">
         <v>155</v>
       </c>
-      <c r="R11" t="s">
-        <v>186</v>
-      </c>
-      <c r="S11" t="s">
-        <v>195</v>
-      </c>
-      <c r="T11" s="14" t="s">
-        <v>198</v>
+      <c r="R11" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="U11" s="4" t="s">
         <v>69</v>
@@ -2480,10 +2568,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
         <v>36</v>
@@ -2492,7 +2580,7 @@
         <v>25</v>
       </c>
       <c r="G12">
-        <v>2012</v>
+        <v>2023</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -2501,37 +2589,37 @@
         <v>66</v>
       </c>
       <c r="J12" s="1">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="K12" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="M12" t="s">
-        <v>199</v>
-      </c>
-      <c r="N12" t="s">
-        <v>201</v>
+        <v>194</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>202</v>
+        <v>1</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>196</v>
       </c>
       <c r="Q12" t="s">
         <v>155</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="S12" t="s">
-        <v>204</v>
-      </c>
-      <c r="T12" s="14" t="s">
-        <v>203</v>
+      <c r="S12" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="T12" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>69</v>
@@ -2542,19 +2630,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G13">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -2563,37 +2651,37 @@
         <v>66</v>
       </c>
       <c r="J13" s="1">
-        <v>0.85</v>
+        <v>0.94</v>
       </c>
       <c r="K13" s="5">
         <v>6</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="M13" t="s">
-        <v>214</v>
-      </c>
-      <c r="N13" t="s">
-        <v>185</v>
+        <v>200</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" t="s">
-        <v>185</v>
+        <v>0</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>202</v>
       </c>
       <c r="Q13" t="s">
-        <v>154</v>
-      </c>
-      <c r="R13" t="s">
-        <v>156</v>
-      </c>
-      <c r="S13" t="s">
-        <v>215</v>
-      </c>
-      <c r="T13" s="14" t="s">
-        <v>216</v>
+        <v>155</v>
+      </c>
+      <c r="R13" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="S13" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>69</v>
@@ -2604,58 +2692,58 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="K14" s="5">
         <v>6</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="M14" t="s">
-        <v>218</v>
-      </c>
-      <c r="N14" t="s">
+        <v>213</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="N14" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="16" t="s">
         <v>185</v>
       </c>
       <c r="Q14" t="s">
         <v>154</v>
       </c>
-      <c r="R14" t="s">
-        <v>221</v>
-      </c>
-      <c r="S14" t="s">
-        <v>219</v>
-      </c>
-      <c r="T14" s="14" t="s">
-        <v>108</v>
+      <c r="R14" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="S14" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="U14" s="4" t="s">
         <v>69</v>
@@ -2666,25 +2754,25 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1">
         <v>0.95</v>
@@ -2693,31 +2781,31 @@
         <v>6</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="M15" t="s">
-        <v>223</v>
-      </c>
-      <c r="N15" t="s">
+        <v>217</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="16" t="s">
         <v>185</v>
       </c>
       <c r="Q15" t="s">
-        <v>155</v>
-      </c>
-      <c r="R15" t="s">
-        <v>155</v>
-      </c>
-      <c r="S15" t="s">
-        <v>224</v>
-      </c>
-      <c r="T15" s="14" t="s">
-        <v>225</v>
+        <v>154</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>69</v>
@@ -2728,19 +2816,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G16">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -2749,37 +2837,37 @@
         <v>66</v>
       </c>
       <c r="J16" s="1">
-        <v>0.84</v>
+        <v>0.95</v>
       </c>
       <c r="K16" s="5">
         <v>6</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="M16" t="s">
-        <v>231</v>
-      </c>
-      <c r="N16" t="s">
+        <v>222</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="N16" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16" t="s">
-        <v>233</v>
+        <v>0</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="Q16" t="s">
         <v>155</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S16" t="s">
-        <v>234</v>
-      </c>
-      <c r="T16" s="14" t="s">
-        <v>232</v>
+      <c r="S16" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>69</v>
@@ -2790,58 +2878,58 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G17">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>
       </c>
       <c r="I17" t="s">
-        <v>248</v>
+        <v>66</v>
       </c>
       <c r="J17" s="1">
-        <v>0.98</v>
+        <v>0.84</v>
       </c>
       <c r="K17" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="M17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N17" t="s">
+        <v>230</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="N17" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>247</v>
+        <v>1</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="Q17" t="s">
         <v>155</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S17" t="s">
-        <v>245</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>246</v>
+      <c r="S17" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>232</v>
       </c>
       <c r="U17" s="4" t="s">
         <v>69</v>
@@ -2852,58 +2940,58 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G18">
-        <v>2023</v>
+        <v>2015</v>
       </c>
       <c r="H18" t="s">
         <v>38</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>248</v>
       </c>
       <c r="J18" s="1">
         <v>0.98</v>
       </c>
       <c r="K18" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="M18" t="s">
-        <v>254</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>255</v>
+        <v>243</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>256</v>
+        <v>0</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="Q18" t="s">
         <v>155</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S18" t="s">
-        <v>258</v>
-      </c>
-      <c r="T18" s="14" t="s">
-        <v>257</v>
+      <c r="S18" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>246</v>
       </c>
       <c r="U18" s="4" t="s">
         <v>69</v>
@@ -2914,7 +3002,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -2923,7 +3011,7 @@
         <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19">
         <v>2023</v>
@@ -2935,37 +3023,37 @@
         <v>66</v>
       </c>
       <c r="J19" s="1">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="K19" s="5">
         <v>6</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="M19" t="s">
-        <v>260</v>
-      </c>
-      <c r="N19" t="s">
-        <v>185</v>
+        <v>253</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>255</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19" t="s">
-        <v>261</v>
+      <c r="P19" s="16" t="s">
+        <v>256</v>
       </c>
       <c r="Q19" t="s">
         <v>155</v>
       </c>
-      <c r="R19" t="s">
-        <v>187</v>
-      </c>
-      <c r="S19" t="s">
-        <v>262</v>
-      </c>
-      <c r="T19" s="14" t="s">
-        <v>263</v>
+      <c r="R19" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="T19" s="13" t="s">
+        <v>257</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>69</v>
@@ -2976,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2985,49 +3073,49 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G20">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J20" s="1">
-        <v>0.98</v>
+        <v>0.6</v>
       </c>
       <c r="K20" s="5">
         <v>6</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="M20" t="s">
-        <v>265</v>
-      </c>
-      <c r="N20" s="15" t="s">
-        <v>266</v>
+        <v>259</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
-      <c r="P20" t="s">
-        <v>267</v>
+      <c r="P20" s="16" t="s">
+        <v>261</v>
       </c>
       <c r="Q20" t="s">
-        <v>154</v>
-      </c>
-      <c r="R20" t="s">
-        <v>156</v>
-      </c>
-      <c r="S20" t="s">
-        <v>268</v>
-      </c>
-      <c r="T20" s="14" t="s">
-        <v>269</v>
+        <v>155</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="S20" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="T20" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="U20" s="4" t="s">
         <v>69</v>
@@ -3038,10 +3126,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -3050,7 +3138,7 @@
         <v>25</v>
       </c>
       <c r="G21">
-        <v>2010</v>
+        <v>2022</v>
       </c>
       <c r="H21" t="s">
         <v>38</v>
@@ -3059,37 +3147,37 @@
         <v>64</v>
       </c>
       <c r="J21" s="1">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="K21" s="5">
         <v>6</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="M21" t="s">
-        <v>271</v>
-      </c>
-      <c r="N21" t="s">
-        <v>185</v>
+        <v>264</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>266</v>
       </c>
       <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>272</v>
+        <v>1</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>267</v>
       </c>
       <c r="Q21" t="s">
-        <v>155</v>
-      </c>
-      <c r="R21" t="s">
-        <v>155</v>
-      </c>
-      <c r="S21" t="s">
-        <v>273</v>
-      </c>
-      <c r="T21" s="14" t="s">
-        <v>109</v>
+        <v>154</v>
+      </c>
+      <c r="R21" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="S21" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="T21" s="13" t="s">
+        <v>269</v>
       </c>
       <c r="U21" s="4" t="s">
         <v>69</v>
@@ -3100,58 +3188,58 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G22">
-        <v>1978</v>
+        <v>2010</v>
       </c>
       <c r="H22" t="s">
         <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J22" s="1">
-        <v>0.85</v>
+        <v>0.96</v>
       </c>
       <c r="K22" s="5">
         <v>6</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="M22" t="s">
-        <v>294</v>
-      </c>
-      <c r="N22" t="s">
+        <v>270</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N22" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" t="s">
-        <v>296</v>
+      <c r="P22" s="16" t="s">
+        <v>272</v>
       </c>
       <c r="Q22" t="s">
         <v>155</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S22" t="s">
-        <v>295</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>297</v>
+      <c r="S22" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="T22" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>69</v>
@@ -3162,19 +3250,19 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23">
-        <v>2023</v>
+        <v>1978</v>
       </c>
       <c r="H23" t="s">
         <v>38</v>
@@ -3189,31 +3277,31 @@
         <v>6</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="M23" t="s">
-        <v>300</v>
-      </c>
-      <c r="N23" s="15" t="s">
-        <v>313</v>
+        <v>293</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23" t="s">
-        <v>299</v>
+      <c r="P23" s="16" t="s">
+        <v>296</v>
       </c>
       <c r="Q23" t="s">
-        <v>153</v>
-      </c>
-      <c r="R23" t="s">
-        <v>186</v>
-      </c>
-      <c r="S23" t="s">
-        <v>301</v>
-      </c>
-      <c r="T23" s="14" t="s">
-        <v>302</v>
+        <v>155</v>
+      </c>
+      <c r="R23" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="T23" s="13" t="s">
+        <v>297</v>
       </c>
       <c r="U23" s="4" t="s">
         <v>69</v>
@@ -3224,16 +3312,16 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G24">
         <v>2023</v>
@@ -3242,40 +3330,40 @@
         <v>38</v>
       </c>
       <c r="I24" t="s">
-        <v>248</v>
+        <v>66</v>
       </c>
       <c r="J24" s="1">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K24" s="5">
+        <v>6</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="O24">
         <v>0</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="M24" t="s">
-        <v>307</v>
-      </c>
-      <c r="N24" t="s">
-        <v>185</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24" t="s">
-        <v>309</v>
+      <c r="P24" s="16" t="s">
+        <v>299</v>
       </c>
       <c r="Q24" t="s">
-        <v>155</v>
-      </c>
-      <c r="R24" t="s">
-        <v>155</v>
-      </c>
-      <c r="S24" t="s">
-        <v>224</v>
-      </c>
-      <c r="T24" s="14" t="s">
-        <v>310</v>
+        <v>153</v>
+      </c>
+      <c r="R24" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="S24" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="T24" s="13" t="s">
+        <v>302</v>
       </c>
       <c r="U24" s="4" t="s">
         <v>69</v>
@@ -3286,61 +3374,61 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>317</v>
+        <v>63</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>248</v>
       </c>
       <c r="J25" s="1">
-        <v>0.65</v>
+        <v>0.9</v>
       </c>
       <c r="K25" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="M25" t="s">
-        <v>360</v>
-      </c>
-      <c r="N25" s="15" t="s">
-        <v>312</v>
+        <v>308</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25" t="s">
-        <v>185</v>
+        <v>1</v>
+      </c>
+      <c r="P25" s="16" t="s">
+        <v>309</v>
       </c>
       <c r="Q25" t="s">
-        <v>153</v>
-      </c>
-      <c r="R25" t="s">
-        <v>156</v>
-      </c>
-      <c r="S25" t="s">
-        <v>316</v>
+        <v>155</v>
+      </c>
+      <c r="R25" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>224</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>314</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
@@ -3348,25 +3436,25 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
         <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G26">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="H26" t="s">
         <v>38</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J26" s="1">
         <v>0.65</v>
@@ -3375,34 +3463,34 @@
         <v>2</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="M26" t="s">
-        <v>318</v>
-      </c>
-      <c r="N26" s="15" t="s">
-        <v>224</v>
+        <v>311</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>312</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="16" t="s">
         <v>185</v>
       </c>
       <c r="Q26" t="s">
-        <v>155</v>
-      </c>
-      <c r="R26" t="s">
-        <v>155</v>
-      </c>
-      <c r="S26" t="s">
-        <v>320</v>
+        <v>153</v>
+      </c>
+      <c r="R26" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="S26" s="18" t="s">
+        <v>316</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
@@ -3410,25 +3498,25 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
         <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G27">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H27" t="s">
         <v>38</v>
       </c>
       <c r="I27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J27" s="1">
         <v>0.65</v>
@@ -3437,34 +3525,34 @@
         <v>2</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="N27" t="s">
-        <v>185</v>
+        <v>321</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>224</v>
       </c>
       <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="16" t="s">
         <v>185</v>
       </c>
       <c r="Q27" t="s">
         <v>155</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S27" t="s">
-        <v>329</v>
+      <c r="S27" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
@@ -3472,19 +3560,19 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F28" t="s">
         <v>25</v>
       </c>
       <c r="G28">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H28" t="s">
         <v>38</v>
@@ -3493,216 +3581,249 @@
         <v>64</v>
       </c>
       <c r="J28" s="1">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="K28" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M28" t="s">
-        <v>332</v>
-      </c>
-      <c r="N28" s="15" t="s">
-        <v>343</v>
+        <v>326</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28" t="s">
-        <v>342</v>
+        <v>1</v>
+      </c>
+      <c r="P28" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="Q28" t="s">
         <v>155</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R28" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S28" t="s">
-        <v>341</v>
+      <c r="S28" s="18" t="s">
+        <v>329</v>
       </c>
       <c r="T28" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="U28" s="3"/>
+        <v>328</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G29">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="H29" t="s">
         <v>38</v>
       </c>
       <c r="I29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J29" s="1">
         <v>0.8</v>
       </c>
       <c r="K29" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="M29" t="s">
-        <v>335</v>
-      </c>
-      <c r="N29" s="15" t="s">
-        <v>75</v>
+        <v>330</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>343</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="P29" t="s">
-        <v>340</v>
+      <c r="P29" s="16" t="s">
+        <v>342</v>
       </c>
       <c r="Q29" t="s">
         <v>155</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S29" t="s">
-        <v>339</v>
+      <c r="S29" s="18" t="s">
+        <v>341</v>
       </c>
       <c r="T29" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>337</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="U29" s="3"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" t="s">
-        <v>368</v>
-      </c>
-      <c r="G30" s="16">
-        <v>2023</v>
-      </c>
-      <c r="H30" t="s">
-        <v>38</v>
+      <c r="B30">
+        <v>28</v>
       </c>
       <c r="J30" s="1"/>
-      <c r="K30" s="5">
-        <v>3</v>
-      </c>
-      <c r="L30" t="s">
-        <v>344</v>
-      </c>
-      <c r="M30" t="s">
-        <v>360</v>
-      </c>
-      <c r="N30" s="15"/>
-      <c r="T30" s="6" t="s">
-        <v>315</v>
-      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="14"/>
+      <c r="P30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="19"/>
       <c r="U30" s="3"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>29</v>
       </c>
+      <c r="C31" t="s">
+        <v>336</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
       <c r="E31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="16">
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31">
         <v>2023</v>
       </c>
       <c r="H31" t="s">
         <v>38</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="5"/>
-      <c r="L31" t="s">
-        <v>345</v>
-      </c>
-      <c r="M31" t="s">
-        <v>361</v>
-      </c>
-      <c r="N31" s="15"/>
-      <c r="T31" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="U31" s="3"/>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K31" s="5">
+        <v>4</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>155</v>
+      </c>
+      <c r="R31" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="S31" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="T31" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B32">
-        <v>30</v>
+      <c r="C32" t="s">
+        <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="16">
+        <v>368</v>
+      </c>
+      <c r="G32" s="15">
         <v>2023</v>
       </c>
       <c r="H32" t="s">
         <v>38</v>
       </c>
-      <c r="L32" t="s">
-        <v>346</v>
-      </c>
-      <c r="M32" t="s">
-        <v>362</v>
-      </c>
-      <c r="T32" s="14" t="s">
-        <v>369</v>
-      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="5">
+        <v>3</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M32" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="N32" s="14"/>
+      <c r="P32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="U32" s="3"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="16">
-        <v>2022</v>
+      <c r="G33" s="15">
+        <v>2023</v>
       </c>
       <c r="H33" t="s">
         <v>38</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="5"/>
-      <c r="L33" t="s">
-        <v>347</v>
-      </c>
-      <c r="M33" t="s">
-        <v>95</v>
-      </c>
-      <c r="N33" s="15"/>
-      <c r="T33" s="6" t="s">
-        <v>97</v>
+      <c r="L33" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="M33" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="N33" s="14"/>
+      <c r="P33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="13" t="s">
+        <v>354</v>
       </c>
       <c r="U33" s="3"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="15">
         <v>2023</v>
       </c>
       <c r="H34" t="s">
@@ -3710,184 +3831,252 @@
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="5"/>
-      <c r="L34" t="s">
-        <v>348</v>
-      </c>
-      <c r="M34" t="s">
-        <v>363</v>
-      </c>
-      <c r="N34" s="15"/>
-      <c r="T34" s="6" t="s">
-        <v>355</v>
+      <c r="L34" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M34" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="N34" s="14"/>
+      <c r="P34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="13" t="s">
+        <v>369</v>
       </c>
       <c r="U34" s="3"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="16">
-        <v>2019</v>
+      <c r="G35" s="15">
+        <v>2022</v>
       </c>
       <c r="H35" t="s">
         <v>38</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="5"/>
-      <c r="L35" t="s">
-        <v>349</v>
-      </c>
-      <c r="M35" t="s">
-        <v>364</v>
-      </c>
-      <c r="N35" s="15"/>
-      <c r="T35" s="6" t="s">
-        <v>356</v>
+      <c r="L35" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="M35" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="N35" s="14"/>
+      <c r="P35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="U35" s="3"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="16">
-        <v>2020</v>
+      <c r="G36" s="15">
+        <v>2023</v>
       </c>
       <c r="H36" t="s">
         <v>38</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="5"/>
-      <c r="L36" t="s">
-        <v>350</v>
-      </c>
-      <c r="M36" t="s">
-        <v>365</v>
-      </c>
-      <c r="N36" s="15"/>
-      <c r="T36" s="6" t="s">
-        <v>357</v>
+      <c r="L36" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="N36" s="14"/>
+      <c r="P36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="13" t="s">
+        <v>355</v>
       </c>
       <c r="U36" s="3"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="16">
-        <v>2015</v>
+      <c r="G37" s="15">
+        <v>2019</v>
       </c>
       <c r="H37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="5"/>
-      <c r="L37" t="s">
-        <v>351</v>
-      </c>
-      <c r="M37" t="s">
-        <v>366</v>
-      </c>
-      <c r="N37" s="15"/>
-      <c r="T37" s="6" t="s">
-        <v>358</v>
+      <c r="L37" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M37" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="N37" s="14"/>
+      <c r="P37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="13" t="s">
+        <v>356</v>
       </c>
       <c r="U37" s="3"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="16">
-        <v>2022</v>
+      <c r="G38" s="15">
+        <v>2020</v>
       </c>
       <c r="H38" t="s">
         <v>38</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="5"/>
-      <c r="L38" t="s">
-        <v>352</v>
-      </c>
-      <c r="M38" t="s">
-        <v>367</v>
-      </c>
-      <c r="N38" s="15"/>
-      <c r="T38" s="6" t="s">
-        <v>359</v>
+      <c r="L38" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="N38" s="14"/>
+      <c r="P38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="13" t="s">
+        <v>357</v>
       </c>
       <c r="U38" s="3"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
       </c>
-      <c r="G39" s="16">
-        <v>2012</v>
+      <c r="G39" s="15">
+        <v>2015</v>
       </c>
       <c r="H39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="5"/>
-      <c r="L39" t="s">
-        <v>353</v>
-      </c>
-      <c r="M39" t="s">
-        <v>199</v>
-      </c>
-      <c r="N39" s="15"/>
-      <c r="T39" s="6" t="s">
-        <v>203</v>
+      <c r="L39" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="N39" s="14"/>
+      <c r="P39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="13" t="s">
+        <v>358</v>
       </c>
       <c r="U39" s="3"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" s="15">
+        <v>2022</v>
+      </c>
+      <c r="H40" t="s">
+        <v>38</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="2"/>
-      <c r="N40" s="15"/>
+      <c r="L40" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="N40" s="14"/>
+      <c r="P40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="13" t="s">
+        <v>359</v>
+      </c>
       <c r="U40" s="3"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="15">
+        <v>2012</v>
+      </c>
+      <c r="H41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="5"/>
+      <c r="L41" t="s">
+        <v>353</v>
+      </c>
+      <c r="M41" t="s">
+        <v>199</v>
+      </c>
+      <c r="N41" s="14"/>
+      <c r="T41" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="U41" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B3:U40">
-    <cfRule type="expression" dxfId="11" priority="3">
+  <conditionalFormatting sqref="B3:U8 C10:U29 C31:U41 B9:B31">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>$E3="Duplicate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E39">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="E3:E8 E10:E29 E31:E41">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Analysed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
       <formula>"ToDo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I31 I33:I34">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="I35:I36 I3:I8 I10:I29 I31:I33">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"None"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33:J34 J3:J31">
+  <conditionalFormatting sqref="J35:J36 J3:J8 J10:J29 J31:J33">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3901,39 +4090,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N31 N33:N34">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+  <conditionalFormatting sqref="N35:N36 N3:N8 N10:N29 N31:N33">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="notEqual">
       <formula>"not specified"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O31 O33:O34">
-    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
+  <conditionalFormatting sqref="O35:O36 O3:O8 O10:O29 O31:O33">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P31 P33:P34">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+  <conditionalFormatting sqref="P35:P36 P3:P8 P10:P29 P31:P33">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:R31 Q33:R34">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="notEqual">
+  <conditionalFormatting sqref="Q35:R36 Q3:R8 Q10:R29 Q31:R33">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="notEqual">
       <formula>"Not mentioned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"not mentioned"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B34:B41">
+    <cfRule type="expression" dxfId="12" priority="25">
+      <formula>$E33="Duplicate"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B31 B33 B35 B37 B39" xr:uid="{A8AF43FC-C864-0442-BE4D-1BD3B99797F0}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D33:D34 D3:D31" xr:uid="{DE81B6F3-8CEE-BE43-8C07-AF5DC780196D}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35:D36 D3:D8 D31:D33 D10:D29" xr:uid="{DE81B6F3-8CEE-BE43-8C07-AF5DC780196D}">
       <formula1>0</formula1>
       <formula2>5</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B31 B33:B41" xr:uid="{A8AF43FC-C864-0442-BE4D-1BD3B99797F0}">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -3949,43 +4143,43 @@
     <hyperlink ref="T7" r:id="rId10" xr:uid="{18E5466D-8E21-C247-971B-D821BE670D8F}"/>
     <hyperlink ref="U8" r:id="rId11" xr:uid="{62D0841C-16FA-6543-BA4C-FAECF857B010}"/>
     <hyperlink ref="T8" r:id="rId12" xr:uid="{00DB0367-9D6E-4547-95D0-96A94B8A5A93}"/>
-    <hyperlink ref="U9" r:id="rId13" xr:uid="{5F1B7AA2-AB53-B146-A204-C7F830508B36}"/>
-    <hyperlink ref="U10" r:id="rId14" xr:uid="{3E6CBF67-FB43-F04E-AAD6-386B2E32BB6A}"/>
-    <hyperlink ref="U11:U24" r:id="rId15" display="https://drive.google.com/file/d/1wbAdCvaoGtQI5B9cn7DfkgudKKb9hup6/view?usp=drive_link" xr:uid="{A8D126F0-00FC-5345-B522-A248592AFEAA}"/>
-    <hyperlink ref="T10" r:id="rId16" tooltip="Persistent link using digital object identifier" xr:uid="{685C278F-F99D-5742-A8B7-26B6BFB0EB24}"/>
-    <hyperlink ref="T11" r:id="rId17" xr:uid="{7ECDFC46-5F0C-CE44-9950-5CACDC2CF1D4}"/>
-    <hyperlink ref="T12" r:id="rId18" xr:uid="{A0BF8156-9938-3146-8233-9114FE8D32D2}"/>
-    <hyperlink ref="T13" r:id="rId19" xr:uid="{035DF826-1461-0640-8A7B-5D225F15011C}"/>
-    <hyperlink ref="T14" r:id="rId20" xr:uid="{6AD489C8-906C-7741-9842-F838D7E79EEB}"/>
-    <hyperlink ref="T15" r:id="rId21" xr:uid="{CA3CFD41-4343-BF47-BDBD-E6941AB200A3}"/>
-    <hyperlink ref="T16" r:id="rId22" xr:uid="{DD2FF52B-8D35-A44E-B0ED-45D5D61D0F07}"/>
-    <hyperlink ref="T17" r:id="rId23" xr:uid="{51F7187F-5358-2849-8472-7C3E4E859657}"/>
-    <hyperlink ref="T18" r:id="rId24" xr:uid="{029ED567-C070-B34C-B6D7-D80577E39992}"/>
-    <hyperlink ref="T19" r:id="rId25" xr:uid="{A7329540-65FD-1849-84D2-9244B1BD561A}"/>
-    <hyperlink ref="T20" r:id="rId26" xr:uid="{6A99BFD4-BAB3-7A45-9A88-C5E85FDFF0C8}"/>
-    <hyperlink ref="T21" r:id="rId27" xr:uid="{04A2209A-C01E-4345-AC8F-8B28470D961F}"/>
-    <hyperlink ref="T22" r:id="rId28" xr:uid="{8C5C6103-3A84-CD4B-B0E4-AFB6CBE6268E}"/>
-    <hyperlink ref="T23" r:id="rId29" xr:uid="{4E874567-21A8-234D-ABB7-163AB8D80682}"/>
-    <hyperlink ref="T24" r:id="rId30" xr:uid="{D8F31D70-FEFF-F846-A7B5-58B69D6348ED}"/>
-    <hyperlink ref="U25" r:id="rId31" xr:uid="{2EE5E883-FCE4-8C42-94BC-7A922E62DC65}"/>
-    <hyperlink ref="T25" r:id="rId32" xr:uid="{B475C20A-2E9C-0C4D-B7B7-02C4E5864019}"/>
-    <hyperlink ref="U26" r:id="rId33" xr:uid="{A9EF7319-5B1C-D74E-A561-0DD548530505}"/>
-    <hyperlink ref="T26" r:id="rId34" xr:uid="{CD1BA2B8-9D7A-E549-8FAE-C43DAA1D1D10}"/>
-    <hyperlink ref="U27" r:id="rId35" xr:uid="{51AB83C7-1D02-3D46-8BB5-79D8553CEE32}"/>
-    <hyperlink ref="T27" r:id="rId36" xr:uid="{E9B28FC3-0E80-7645-879C-F52BF29A88F8}"/>
-    <hyperlink ref="T28" r:id="rId37" xr:uid="{A89A9514-5C6D-C64F-8A1B-9355F32E3BF0}"/>
-    <hyperlink ref="U29" r:id="rId38" xr:uid="{4C1F5746-7BAC-484E-A22B-6A77AC8DA912}"/>
-    <hyperlink ref="T29" r:id="rId39" xr:uid="{6E76C6C8-A0B3-A947-8EC9-08753C886A4E}"/>
-    <hyperlink ref="T30" r:id="rId40" xr:uid="{6DE56EDE-B45B-4644-88EA-B8C727147F57}"/>
-    <hyperlink ref="T31" r:id="rId41" xr:uid="{41811598-B0D3-284C-823E-90847AEB2FFC}"/>
-    <hyperlink ref="T33" r:id="rId42" xr:uid="{257D29D1-00B6-6245-8E48-C21CBA9AAEE9}"/>
-    <hyperlink ref="T34" r:id="rId43" xr:uid="{40460462-43F5-3841-BDAB-4F24C2079333}"/>
-    <hyperlink ref="T35" r:id="rId44" xr:uid="{D8D7FB97-5DE1-6940-943F-10C1648DCFEB}"/>
-    <hyperlink ref="T36" r:id="rId45" xr:uid="{5D7A87F1-9345-D64C-B06C-143CE1A13E22}"/>
-    <hyperlink ref="T37" r:id="rId46" xr:uid="{D2B37ECC-4B24-6343-B690-9B9DA0928236}"/>
-    <hyperlink ref="T38" r:id="rId47" xr:uid="{918EF093-4CED-CB4D-8E8C-4AB5E287CD8C}"/>
-    <hyperlink ref="T39" r:id="rId48" xr:uid="{79528344-EEF3-934D-BD0A-EC8259780C9E}"/>
-    <hyperlink ref="T32" r:id="rId49" xr:uid="{A7572C3C-CB17-7E44-BF57-E5CF720D86E9}"/>
+    <hyperlink ref="U10" r:id="rId13" xr:uid="{5F1B7AA2-AB53-B146-A204-C7F830508B36}"/>
+    <hyperlink ref="U11" r:id="rId14" xr:uid="{3E6CBF67-FB43-F04E-AAD6-386B2E32BB6A}"/>
+    <hyperlink ref="U12:U25" r:id="rId15" display="https://drive.google.com/file/d/1wbAdCvaoGtQI5B9cn7DfkgudKKb9hup6/view?usp=drive_link" xr:uid="{A8D126F0-00FC-5345-B522-A248592AFEAA}"/>
+    <hyperlink ref="T11" r:id="rId16" tooltip="Persistent link using digital object identifier" xr:uid="{685C278F-F99D-5742-A8B7-26B6BFB0EB24}"/>
+    <hyperlink ref="T12" r:id="rId17" xr:uid="{7ECDFC46-5F0C-CE44-9950-5CACDC2CF1D4}"/>
+    <hyperlink ref="T13" r:id="rId18" xr:uid="{A0BF8156-9938-3146-8233-9114FE8D32D2}"/>
+    <hyperlink ref="T14" r:id="rId19" xr:uid="{035DF826-1461-0640-8A7B-5D225F15011C}"/>
+    <hyperlink ref="T15" r:id="rId20" xr:uid="{6AD489C8-906C-7741-9842-F838D7E79EEB}"/>
+    <hyperlink ref="T16" r:id="rId21" xr:uid="{CA3CFD41-4343-BF47-BDBD-E6941AB200A3}"/>
+    <hyperlink ref="T17" r:id="rId22" xr:uid="{DD2FF52B-8D35-A44E-B0ED-45D5D61D0F07}"/>
+    <hyperlink ref="T18" r:id="rId23" xr:uid="{51F7187F-5358-2849-8472-7C3E4E859657}"/>
+    <hyperlink ref="T19" r:id="rId24" xr:uid="{029ED567-C070-B34C-B6D7-D80577E39992}"/>
+    <hyperlink ref="T20" r:id="rId25" xr:uid="{A7329540-65FD-1849-84D2-9244B1BD561A}"/>
+    <hyperlink ref="T21" r:id="rId26" xr:uid="{6A99BFD4-BAB3-7A45-9A88-C5E85FDFF0C8}"/>
+    <hyperlink ref="T22" r:id="rId27" xr:uid="{04A2209A-C01E-4345-AC8F-8B28470D961F}"/>
+    <hyperlink ref="T23" r:id="rId28" xr:uid="{8C5C6103-3A84-CD4B-B0E4-AFB6CBE6268E}"/>
+    <hyperlink ref="T24" r:id="rId29" xr:uid="{4E874567-21A8-234D-ABB7-163AB8D80682}"/>
+    <hyperlink ref="T25" r:id="rId30" xr:uid="{D8F31D70-FEFF-F846-A7B5-58B69D6348ED}"/>
+    <hyperlink ref="U26" r:id="rId31" xr:uid="{2EE5E883-FCE4-8C42-94BC-7A922E62DC65}"/>
+    <hyperlink ref="T26" r:id="rId32" xr:uid="{B475C20A-2E9C-0C4D-B7B7-02C4E5864019}"/>
+    <hyperlink ref="U27" r:id="rId33" xr:uid="{A9EF7319-5B1C-D74E-A561-0DD548530505}"/>
+    <hyperlink ref="T27" r:id="rId34" xr:uid="{CD1BA2B8-9D7A-E549-8FAE-C43DAA1D1D10}"/>
+    <hyperlink ref="U28" r:id="rId35" xr:uid="{51AB83C7-1D02-3D46-8BB5-79D8553CEE32}"/>
+    <hyperlink ref="T28" r:id="rId36" xr:uid="{E9B28FC3-0E80-7645-879C-F52BF29A88F8}"/>
+    <hyperlink ref="T29" r:id="rId37" xr:uid="{A89A9514-5C6D-C64F-8A1B-9355F32E3BF0}"/>
+    <hyperlink ref="U31" r:id="rId38" xr:uid="{4C1F5746-7BAC-484E-A22B-6A77AC8DA912}"/>
+    <hyperlink ref="T31" r:id="rId39" xr:uid="{6E76C6C8-A0B3-A947-8EC9-08753C886A4E}"/>
+    <hyperlink ref="T32" r:id="rId40" xr:uid="{6DE56EDE-B45B-4644-88EA-B8C727147F57}"/>
+    <hyperlink ref="T33" r:id="rId41" xr:uid="{41811598-B0D3-284C-823E-90847AEB2FFC}"/>
+    <hyperlink ref="T35" r:id="rId42" xr:uid="{257D29D1-00B6-6245-8E48-C21CBA9AAEE9}"/>
+    <hyperlink ref="T36" r:id="rId43" xr:uid="{40460462-43F5-3841-BDAB-4F24C2079333}"/>
+    <hyperlink ref="T37" r:id="rId44" xr:uid="{D8D7FB97-5DE1-6940-943F-10C1648DCFEB}"/>
+    <hyperlink ref="T38" r:id="rId45" xr:uid="{5D7A87F1-9345-D64C-B06C-143CE1A13E22}"/>
+    <hyperlink ref="T39" r:id="rId46" xr:uid="{D2B37ECC-4B24-6343-B690-9B9DA0928236}"/>
+    <hyperlink ref="T40" r:id="rId47" xr:uid="{918EF093-4CED-CB4D-8E8C-4AB5E287CD8C}"/>
+    <hyperlink ref="T41" r:id="rId48" xr:uid="{79528344-EEF3-934D-BD0A-EC8259780C9E}"/>
+    <hyperlink ref="T34" r:id="rId49" xr:uid="{A7572C3C-CB17-7E44-BF57-E5CF720D86E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4008,7 +4202,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J33:J34 J3:J31</xm:sqref>
+          <xm:sqref>J35:J36 J3:J8 J10:J29 J31:J33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4018,43 +4212,43 @@
           <x14:formula1>
             <xm:f>factors!$C$3:$C$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F33:F34 F3:F31</xm:sqref>
+          <xm:sqref>F35:F36 F3:F8 F31:F33 F10:F29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{566B1144-F99A-C245-8189-04C656B42A78}">
+          <x14:formula1>
+            <xm:f>factors!$F$3:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>I35:I36 I3:I8 I31:I33 I10:I29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1AA26AE0-EDAD-8C47-ACEB-3F6AE8EEE028}">
+          <x14:formula1>
+            <xm:f>factors!$K$3:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q35:Q36 Q3:Q8 Q31:Q33 Q10:Q29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBAE5E32-2C54-BA45-86E5-09D8CE417A28}">
+          <x14:formula1>
+            <xm:f>factors!$G$3:$G$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>N35:N36 N3:N8 N31:N33 N10:N29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{745EE373-4BD2-1042-AADC-7EDFB98FA266}">
+          <x14:formula1>
+            <xm:f>factors!$L$3:$L$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>R35:R36 R3:R8 R31:R33 R10:R29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{497BC3DD-CEC8-2747-860E-683E9AB8EA62}">
           <x14:formula1>
             <xm:f>factors!$D$3:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E40</xm:sqref>
+          <xm:sqref>E3:E8 E31:E41 E10:E29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F2C01858-56B7-724A-B24C-A857D3030B5A}">
           <x14:formula1>
             <xm:f>factors!$E$3:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{566B1144-F99A-C245-8189-04C656B42A78}">
-          <x14:formula1>
-            <xm:f>factors!$F$3:$F$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>I33:I34 I3:I31</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1AA26AE0-EDAD-8C47-ACEB-3F6AE8EEE028}">
-          <x14:formula1>
-            <xm:f>factors!$K$3:$K$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q33:Q34 Q3:Q31</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBAE5E32-2C54-BA45-86E5-09D8CE417A28}">
-          <x14:formula1>
-            <xm:f>factors!$G$3:$G$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>N33:N34 N3:N31</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{745EE373-4BD2-1042-AADC-7EDFB98FA266}">
-          <x14:formula1>
-            <xm:f>factors!$L$3:$L$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>R33:R34 R3:R31</xm:sqref>
+          <xm:sqref>H3:H8 H31:H41 H10:H29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5231,7 +5425,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:C54">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>COUNTIF($C$3:$C3,$C3)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
2024-01-17 progress on methods section
</commit_message>
<xml_diff>
--- a/src/data/raw/2024-01-09_review_papers.xlsx
+++ b/src/data/raw/2024-01-09_review_papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lex/Workspace/phd-research-ucc/repositories/mrs-systematic-analysis/src/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB3C55-6B27-2644-8B94-04EA24458410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2EB30E-FD0E-0845-84A4-728CB33E73D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
   </bookViews>
@@ -1248,7 +1248,7 @@
       <alignment horizontal="fill" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1273,10 +1273,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1284,129 +1280,7 @@
     <cellStyle name="Style 1" xfId="2" xr:uid="{AD703E83-2422-144D-99A8-2ADC57964367}"/>
     <cellStyle name="Style 2" xfId="3" xr:uid="{B9FF1B68-E23A-3C40-85DE-B173152847B9}"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1455,16 +1329,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -1491,11 +1355,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1506,6 +1370,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1615,18 +1489,18 @@
     <tableColumn id="7" xr3:uid="{B5956E56-EA0C-C544-81E9-95D5F85516CE}" name="year"/>
     <tableColumn id="8" xr3:uid="{1D433107-5A8B-4B40-8584-1024473C053A}" name="type"/>
     <tableColumn id="9" xr3:uid="{28A710C7-54CD-BC4D-A29E-7C74FFEB5F42}" name="domain"/>
-    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="33"/>
-    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="19"/>
     <tableColumn id="17" xr3:uid="{5A2B4EE5-BF86-7042-97F7-E54C28D22FA9}" name="covid19"/>
-    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="31"/>
+    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="18"/>
     <tableColumn id="19" xr3:uid="{E63FEC1A-8B57-1B47-AAEC-C5489A7E23BF}" name="coi"/>
-    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="30"/>
-    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="29"/>
-    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="17"/>
+    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="16"/>
+    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1636,7 +1510,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}" name="Table2" displayName="Table2" ref="B2:F46" totalsRowShown="0">
   <autoFilter ref="B2:F46" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{E697A4C6-CB50-0449-AD63-6ACBEE53E663}" name="local_ref"/>
     <tableColumn id="3" xr3:uid="{53E59951-C7CE-0740-917C-0D957BB1897C}" name="ref_url"/>
     <tableColumn id="4" xr3:uid="{1E16B457-6000-4743-9439-9D6865E34250}" name="ref_comment"/>
@@ -2431,12 +2305,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="5"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="16"/>
       <c r="N9" s="14"/>
-      <c r="P9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="19"/>
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
@@ -2473,7 +2342,7 @@
       <c r="L10" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" t="s">
         <v>183</v>
       </c>
       <c r="N10" s="14" t="s">
@@ -2482,16 +2351,16 @@
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P10" t="s">
         <v>185</v>
       </c>
       <c r="Q10" t="s">
         <v>154</v>
       </c>
-      <c r="R10" s="16" t="s">
+      <c r="R10" t="s">
         <v>187</v>
       </c>
-      <c r="S10" s="18" t="s">
+      <c r="S10" t="s">
         <v>181</v>
       </c>
       <c r="T10" s="13" t="s">
@@ -2535,7 +2404,7 @@
       <c r="L11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" t="s">
         <v>188</v>
       </c>
       <c r="N11" s="14" t="s">
@@ -2544,16 +2413,16 @@
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="P11" t="s">
         <v>190</v>
       </c>
       <c r="Q11" t="s">
         <v>155</v>
       </c>
-      <c r="R11" s="16" t="s">
+      <c r="R11" t="s">
         <v>155</v>
       </c>
-      <c r="S11" s="18" t="s">
+      <c r="S11" t="s">
         <v>191</v>
       </c>
       <c r="T11" s="13" t="s">
@@ -2597,7 +2466,7 @@
       <c r="L12" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" t="s">
         <v>193</v>
       </c>
       <c r="N12" s="14" t="s">
@@ -2606,16 +2475,16 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="P12" t="s">
         <v>196</v>
       </c>
       <c r="Q12" t="s">
         <v>155</v>
       </c>
-      <c r="R12" s="16" t="s">
+      <c r="R12" t="s">
         <v>186</v>
       </c>
-      <c r="S12" s="18" t="s">
+      <c r="S12" t="s">
         <v>195</v>
       </c>
       <c r="T12" s="13" t="s">
@@ -2659,7 +2528,7 @@
       <c r="L13" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" t="s">
         <v>199</v>
       </c>
       <c r="N13" s="14" t="s">
@@ -2668,16 +2537,16 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="P13" t="s">
         <v>202</v>
       </c>
       <c r="Q13" t="s">
         <v>155</v>
       </c>
-      <c r="R13" s="16" t="s">
+      <c r="R13" t="s">
         <v>186</v>
       </c>
-      <c r="S13" s="18" t="s">
+      <c r="S13" t="s">
         <v>204</v>
       </c>
       <c r="T13" s="13" t="s">
@@ -2721,7 +2590,7 @@
       <c r="L14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M14" t="s">
         <v>214</v>
       </c>
       <c r="N14" s="14" t="s">
@@ -2730,16 +2599,16 @@
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" t="s">
         <v>185</v>
       </c>
       <c r="Q14" t="s">
         <v>154</v>
       </c>
-      <c r="R14" s="16" t="s">
+      <c r="R14" t="s">
         <v>156</v>
       </c>
-      <c r="S14" s="18" t="s">
+      <c r="S14" t="s">
         <v>215</v>
       </c>
       <c r="T14" s="13" t="s">
@@ -2783,7 +2652,7 @@
       <c r="L15" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" t="s">
         <v>218</v>
       </c>
       <c r="N15" s="14" t="s">
@@ -2792,16 +2661,16 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="P15" t="s">
         <v>185</v>
       </c>
       <c r="Q15" t="s">
         <v>154</v>
       </c>
-      <c r="R15" s="16" t="s">
+      <c r="R15" t="s">
         <v>221</v>
       </c>
-      <c r="S15" s="18" t="s">
+      <c r="S15" t="s">
         <v>219</v>
       </c>
       <c r="T15" s="13" t="s">
@@ -2845,7 +2714,7 @@
       <c r="L16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" t="s">
         <v>223</v>
       </c>
       <c r="N16" s="14" t="s">
@@ -2854,16 +2723,16 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="16" t="s">
+      <c r="P16" t="s">
         <v>185</v>
       </c>
       <c r="Q16" t="s">
         <v>155</v>
       </c>
-      <c r="R16" s="16" t="s">
+      <c r="R16" t="s">
         <v>155</v>
       </c>
-      <c r="S16" s="18" t="s">
+      <c r="S16" t="s">
         <v>224</v>
       </c>
       <c r="T16" s="13" t="s">
@@ -2907,7 +2776,7 @@
       <c r="L17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" t="s">
         <v>231</v>
       </c>
       <c r="N17" s="14" t="s">
@@ -2916,16 +2785,16 @@
       <c r="O17">
         <v>1</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="P17" t="s">
         <v>233</v>
       </c>
       <c r="Q17" t="s">
         <v>155</v>
       </c>
-      <c r="R17" s="16" t="s">
+      <c r="R17" t="s">
         <v>155</v>
       </c>
-      <c r="S17" s="18" t="s">
+      <c r="S17" t="s">
         <v>234</v>
       </c>
       <c r="T17" s="13" t="s">
@@ -2969,7 +2838,7 @@
       <c r="L18" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" t="s">
         <v>244</v>
       </c>
       <c r="N18" s="14" t="s">
@@ -2978,16 +2847,16 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18" s="16" t="s">
+      <c r="P18" t="s">
         <v>247</v>
       </c>
       <c r="Q18" t="s">
         <v>155</v>
       </c>
-      <c r="R18" s="16" t="s">
+      <c r="R18" t="s">
         <v>155</v>
       </c>
-      <c r="S18" s="18" t="s">
+      <c r="S18" t="s">
         <v>245</v>
       </c>
       <c r="T18" s="13" t="s">
@@ -3031,7 +2900,7 @@
       <c r="L19" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" t="s">
         <v>254</v>
       </c>
       <c r="N19" s="14" t="s">
@@ -3040,16 +2909,16 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19" s="16" t="s">
+      <c r="P19" t="s">
         <v>256</v>
       </c>
       <c r="Q19" t="s">
         <v>155</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="R19" t="s">
         <v>155</v>
       </c>
-      <c r="S19" s="18" t="s">
+      <c r="S19" t="s">
         <v>258</v>
       </c>
       <c r="T19" s="13" t="s">
@@ -3093,7 +2962,7 @@
       <c r="L20" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="M20" t="s">
         <v>260</v>
       </c>
       <c r="N20" s="14" t="s">
@@ -3102,16 +2971,16 @@
       <c r="O20">
         <v>1</v>
       </c>
-      <c r="P20" s="16" t="s">
+      <c r="P20" t="s">
         <v>261</v>
       </c>
       <c r="Q20" t="s">
         <v>155</v>
       </c>
-      <c r="R20" s="16" t="s">
+      <c r="R20" t="s">
         <v>187</v>
       </c>
-      <c r="S20" s="18" t="s">
+      <c r="S20" t="s">
         <v>262</v>
       </c>
       <c r="T20" s="13" t="s">
@@ -3155,7 +3024,7 @@
       <c r="L21" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M21" s="16" t="s">
+      <c r="M21" t="s">
         <v>265</v>
       </c>
       <c r="N21" s="14" t="s">
@@ -3164,16 +3033,16 @@
       <c r="O21">
         <v>1</v>
       </c>
-      <c r="P21" s="16" t="s">
+      <c r="P21" t="s">
         <v>267</v>
       </c>
       <c r="Q21" t="s">
         <v>154</v>
       </c>
-      <c r="R21" s="16" t="s">
+      <c r="R21" t="s">
         <v>156</v>
       </c>
-      <c r="S21" s="18" t="s">
+      <c r="S21" t="s">
         <v>268</v>
       </c>
       <c r="T21" s="13" t="s">
@@ -3217,7 +3086,7 @@
       <c r="L22" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="M22" s="16" t="s">
+      <c r="M22" t="s">
         <v>271</v>
       </c>
       <c r="N22" s="14" t="s">
@@ -3226,16 +3095,16 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" s="16" t="s">
+      <c r="P22" t="s">
         <v>272</v>
       </c>
       <c r="Q22" t="s">
         <v>155</v>
       </c>
-      <c r="R22" s="16" t="s">
+      <c r="R22" t="s">
         <v>155</v>
       </c>
-      <c r="S22" s="18" t="s">
+      <c r="S22" t="s">
         <v>273</v>
       </c>
       <c r="T22" s="13" t="s">
@@ -3279,7 +3148,7 @@
       <c r="L23" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="M23" s="16" t="s">
+      <c r="M23" t="s">
         <v>294</v>
       </c>
       <c r="N23" s="14" t="s">
@@ -3288,16 +3157,16 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23" s="16" t="s">
+      <c r="P23" t="s">
         <v>296</v>
       </c>
       <c r="Q23" t="s">
         <v>155</v>
       </c>
-      <c r="R23" s="16" t="s">
+      <c r="R23" t="s">
         <v>155</v>
       </c>
-      <c r="S23" s="18" t="s">
+      <c r="S23" t="s">
         <v>295</v>
       </c>
       <c r="T23" s="13" t="s">
@@ -3341,7 +3210,7 @@
       <c r="L24" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="M24" s="16" t="s">
+      <c r="M24" t="s">
         <v>300</v>
       </c>
       <c r="N24" s="14" t="s">
@@ -3350,16 +3219,16 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="P24" s="16" t="s">
+      <c r="P24" t="s">
         <v>299</v>
       </c>
       <c r="Q24" t="s">
         <v>153</v>
       </c>
-      <c r="R24" s="16" t="s">
+      <c r="R24" t="s">
         <v>186</v>
       </c>
-      <c r="S24" s="18" t="s">
+      <c r="S24" t="s">
         <v>301</v>
       </c>
       <c r="T24" s="13" t="s">
@@ -3403,7 +3272,7 @@
       <c r="L25" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="M25" t="s">
         <v>307</v>
       </c>
       <c r="N25" s="14" t="s">
@@ -3412,16 +3281,16 @@
       <c r="O25">
         <v>1</v>
       </c>
-      <c r="P25" s="16" t="s">
+      <c r="P25" t="s">
         <v>309</v>
       </c>
       <c r="Q25" t="s">
         <v>155</v>
       </c>
-      <c r="R25" s="16" t="s">
+      <c r="R25" t="s">
         <v>155</v>
       </c>
-      <c r="S25" s="18" t="s">
+      <c r="S25" t="s">
         <v>224</v>
       </c>
       <c r="T25" s="13" t="s">
@@ -3465,7 +3334,7 @@
       <c r="L26" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="M26" s="16" t="s">
+      <c r="M26" t="s">
         <v>360</v>
       </c>
       <c r="N26" s="14" t="s">
@@ -3474,16 +3343,16 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26" s="16" t="s">
+      <c r="P26" t="s">
         <v>185</v>
       </c>
       <c r="Q26" t="s">
         <v>153</v>
       </c>
-      <c r="R26" s="16" t="s">
+      <c r="R26" t="s">
         <v>156</v>
       </c>
-      <c r="S26" s="18" t="s">
+      <c r="S26" t="s">
         <v>316</v>
       </c>
       <c r="T26" s="13" t="s">
@@ -3527,7 +3396,7 @@
       <c r="L27" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="M27" s="16" t="s">
+      <c r="M27" t="s">
         <v>318</v>
       </c>
       <c r="N27" s="14" t="s">
@@ -3536,16 +3405,16 @@
       <c r="O27">
         <v>0</v>
       </c>
-      <c r="P27" s="16" t="s">
+      <c r="P27" t="s">
         <v>185</v>
       </c>
       <c r="Q27" t="s">
         <v>155</v>
       </c>
-      <c r="R27" s="16" t="s">
+      <c r="R27" t="s">
         <v>155</v>
       </c>
-      <c r="S27" s="18" t="s">
+      <c r="S27" t="s">
         <v>320</v>
       </c>
       <c r="T27" s="13" t="s">
@@ -3589,7 +3458,7 @@
       <c r="L28" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="M28" s="17" t="s">
+      <c r="M28" s="2" t="s">
         <v>324</v>
       </c>
       <c r="N28" s="14" t="s">
@@ -3598,16 +3467,16 @@
       <c r="O28">
         <v>1</v>
       </c>
-      <c r="P28" s="16" t="s">
+      <c r="P28" t="s">
         <v>185</v>
       </c>
       <c r="Q28" t="s">
         <v>155</v>
       </c>
-      <c r="R28" s="16" t="s">
+      <c r="R28" t="s">
         <v>155</v>
       </c>
-      <c r="S28" s="18" t="s">
+      <c r="S28" t="s">
         <v>329</v>
       </c>
       <c r="T28" s="13" t="s">
@@ -3651,7 +3520,7 @@
       <c r="L29" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="M29" t="s">
         <v>332</v>
       </c>
       <c r="N29" s="14" t="s">
@@ -3660,16 +3529,16 @@
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="P29" s="16" t="s">
+      <c r="P29" t="s">
         <v>342</v>
       </c>
       <c r="Q29" t="s">
         <v>155</v>
       </c>
-      <c r="R29" s="16" t="s">
+      <c r="R29" t="s">
         <v>155</v>
       </c>
-      <c r="S29" s="18" t="s">
+      <c r="S29" t="s">
         <v>341</v>
       </c>
       <c r="T29" s="13" t="s">
@@ -3684,12 +3553,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="5"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="16"/>
       <c r="N30" s="14"/>
-      <c r="P30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="19"/>
       <c r="U30" s="3"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
@@ -3726,7 +3590,7 @@
       <c r="L31" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M31" t="s">
         <v>335</v>
       </c>
       <c r="N31" s="14" t="s">
@@ -3735,16 +3599,16 @@
       <c r="O31">
         <v>0</v>
       </c>
-      <c r="P31" s="16" t="s">
+      <c r="P31" t="s">
         <v>340</v>
       </c>
       <c r="Q31" t="s">
         <v>155</v>
       </c>
-      <c r="R31" s="16" t="s">
+      <c r="R31" t="s">
         <v>155</v>
       </c>
-      <c r="S31" s="18" t="s">
+      <c r="S31" t="s">
         <v>339</v>
       </c>
       <c r="T31" s="13" t="s">
@@ -3774,13 +3638,10 @@
       <c r="L32" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="M32" s="16" t="s">
+      <c r="M32" t="s">
         <v>360</v>
       </c>
       <c r="N32" s="14"/>
-      <c r="P32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="18"/>
       <c r="T32" s="13" t="s">
         <v>315</v>
       </c>
@@ -3804,13 +3665,10 @@
       <c r="L33" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="M33" s="16" t="s">
+      <c r="M33" t="s">
         <v>361</v>
       </c>
       <c r="N33" s="14"/>
-      <c r="P33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="18"/>
       <c r="T33" s="13" t="s">
         <v>354</v>
       </c>
@@ -3834,13 +3692,10 @@
       <c r="L34" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="M34" s="16" t="s">
+      <c r="M34" t="s">
         <v>362</v>
       </c>
       <c r="N34" s="14"/>
-      <c r="P34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="18"/>
       <c r="T34" s="13" t="s">
         <v>369</v>
       </c>
@@ -3864,13 +3719,10 @@
       <c r="L35" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="M35" t="s">
         <v>95</v>
       </c>
       <c r="N35" s="14"/>
-      <c r="P35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="18"/>
       <c r="T35" s="13" t="s">
         <v>97</v>
       </c>
@@ -3894,13 +3746,10 @@
       <c r="L36" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="M36" s="16" t="s">
+      <c r="M36" t="s">
         <v>363</v>
       </c>
       <c r="N36" s="14"/>
-      <c r="P36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="18"/>
       <c r="T36" s="13" t="s">
         <v>355</v>
       </c>
@@ -3924,13 +3773,10 @@
       <c r="L37" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="M37" s="16" t="s">
+      <c r="M37" t="s">
         <v>364</v>
       </c>
       <c r="N37" s="14"/>
-      <c r="P37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="18"/>
       <c r="T37" s="13" t="s">
         <v>356</v>
       </c>
@@ -3954,13 +3800,10 @@
       <c r="L38" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="M38" s="16" t="s">
+      <c r="M38" t="s">
         <v>365</v>
       </c>
       <c r="N38" s="14"/>
-      <c r="P38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="18"/>
       <c r="T38" s="13" t="s">
         <v>357</v>
       </c>
@@ -3984,13 +3827,10 @@
       <c r="L39" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="M39" s="16" t="s">
+      <c r="M39" t="s">
         <v>366</v>
       </c>
       <c r="N39" s="14"/>
-      <c r="P39" s="16"/>
-      <c r="R39" s="16"/>
-      <c r="S39" s="18"/>
       <c r="T39" s="13" t="s">
         <v>358</v>
       </c>
@@ -4014,13 +3854,10 @@
       <c r="L40" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="M40" s="16" t="s">
+      <c r="M40" t="s">
         <v>367</v>
       </c>
       <c r="N40" s="14"/>
-      <c r="P40" s="16"/>
-      <c r="R40" s="16"/>
-      <c r="S40" s="18"/>
       <c r="T40" s="13" t="s">
         <v>359</v>
       </c>
@@ -4055,24 +3892,29 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B34:B41">
+    <cfRule type="expression" dxfId="12" priority="25">
+      <formula>$E33="Duplicate"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:U8 C10:U29 C31:U41 B9:B31">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$E3="Duplicate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E8 E10:E29 E31:E41">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"ToDo"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Analysed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"ToDo"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:I36 I3:I8 I10:I29 I31:I33">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+  <conditionalFormatting sqref="I3:I8 I10:I29 I31:I33 I35:I36">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"None"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4090,35 +3932,30 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N35:N36 N3:N8 N10:N29 N31:N33">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="notEqual">
+  <conditionalFormatting sqref="N3:N8 N10:N29 N31:N33 N35:N36">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="notEqual">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O35:O36 O3:O8 O10:O29 O31:O33">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+  <conditionalFormatting sqref="O3:O8 O10:O29 O31:O33 O35:O36">
+    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P35:P36 P3:P8 P10:P29 P31:P33">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+  <conditionalFormatting sqref="P3:P8 P10:P29 P31:P33 P35:P36">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q35:R36 Q3:R8 Q10:R29 Q31:R33">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="notEqual">
+  <conditionalFormatting sqref="Q3:R8 Q10:R29 Q31:R33 Q35:R36">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="notEqual">
       <formula>"Not mentioned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>"not mentioned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B41">
-    <cfRule type="expression" dxfId="12" priority="25">
-      <formula>$E33="Duplicate"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -4296,7 +4133,7 @@
   <dimension ref="B2:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="B5" sqref="B5:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4844,6 +4681,7 @@
     <hyperlink ref="D44" r:id="rId36" xr:uid="{54A17B45-9CAF-704A-92DF-92CF3F3F7D13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId37"/>
   </tableParts>
@@ -4867,7 +4705,7 @@
   <dimension ref="B2:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C54"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5425,7 +5263,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:C54">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>COUNTIF($C$3:$C3,$C3)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>